<commit_message>
alles is nagemeten en 75% is ingeleverd
</commit_message>
<xml_diff>
--- a/school/75%.xlsx
+++ b/school/75%.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ptibe-my.sharepoint.com/personal/stan_debakker_leerling_pti_be/Documents/programeren/Arduino/6TWEA/grap-6TWEA/school/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{F8A846CE-0E17-47E4-8763-E58D7D399E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70A758FB-8CF3-4827-B539-303917F2A3F5}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{F8A846CE-0E17-47E4-8763-E58D7D399E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E3120CD-0133-48EC-B7A6-1032EB772C52}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8D02C5D0-9212-4D29-AED6-60E55B7BB112}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">voldoende </t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>alles wat ik heb kunnen testen heb ik getest nog allen enkele sensoren die ik nu nog niet kon testen moet ik nog testen</t>
+  </si>
+  <si>
+    <t>ik ben nu aan het kijken om het "hoofd", lijnsensor en addon kaart te vernieuwen maar ik ga waschijnlijk niet het hoofdbord kunnen vervangen maar meschien al tekenen</t>
+  </si>
+  <si>
+    <t>door te expirimenteren met wifi kan ik het op afstand besturen maar school maakt het wel moeilijker</t>
+  </si>
+  <si>
+    <t>de nieuwe bordjes bestellen maken en testen en mocht ik nog tijd hebben al beginnen met het hoofdbord te tekenen</t>
+  </si>
+  <si>
+    <t>dit vind ik heel moeilijk maar ik werk wel veet thuis</t>
   </si>
 </sst>
 </file>
@@ -646,6 +658,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -968,7 +984,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -997,7 +1013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1006,10 +1022,12 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -1021,7 +1039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -1029,7 +1047,9 @@
       <c r="C4" s="4"/>
       <c r="D4" s="6"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="10"/>
+      <c r="F4" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
@@ -1039,7 +1059,9 @@
       <c r="C5" s="4"/>
       <c r="D5" s="6"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="10"/>
+      <c r="F5" s="10" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
@@ -1054,7 +1076,9 @@
         <v>6</v>
       </c>
       <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="C7" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -1102,12 +1126,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ReferenceId xmlns="a0473d4f-1cca-4074-b684-28dae071d4ec" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1261,17 +1284,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ReferenceId xmlns="a0473d4f-1cca-4074-b684-28dae071d4ec" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94C58001-208F-4438-8A61-90F840F8F010}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E1C4DFE-DBD8-43C6-AD80-6E9A289D5A4B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a0473d4f-1cca-4074-b684-28dae071d4ec"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1295,11 +1321,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E1C4DFE-DBD8-43C6-AD80-6E9A289D5A4B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94C58001-208F-4438-8A61-90F840F8F010}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a0473d4f-1cca-4074-b684-28dae071d4ec"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>